<commit_message>
Mise à jour du 17-12-2021
</commit_message>
<xml_diff>
--- a/Doc/Ma Finance.xlsx
+++ b/Doc/Ma Finance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrateur\Desktop\workspace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\amesika\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D514E25-808B-42B9-93F0-00B5747637D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840D5075-5094-4AE1-B168-8AADCC89AA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -889,6 +889,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -897,27 +918,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2063,10 +2063,10 @@
       <c r="Z3" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="AB3" s="86" t="s">
+      <c r="AB3" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="AC3" s="87"/>
+      <c r="AC3" s="94"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
@@ -2202,8 +2202,8 @@
       </c>
     </row>
     <row r="7" spans="1:29" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AB7" s="88"/>
-      <c r="AC7" s="88"/>
+      <c r="AB7" s="87"/>
+      <c r="AC7" s="87"/>
     </row>
     <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="61" t="s">
@@ -2269,11 +2269,11 @@
         <v>2160</v>
       </c>
       <c r="Z8" s="28"/>
-      <c r="AB8" s="89">
+      <c r="AB8" s="90">
         <f t="shared" si="0"/>
         <v>27120</v>
       </c>
-      <c r="AC8" s="90"/>
+      <c r="AC8" s="91"/>
     </row>
     <row r="9" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
@@ -2302,8 +2302,8 @@
       <c r="X9" s="12"/>
       <c r="Y9" s="12"/>
       <c r="Z9" s="12"/>
-      <c r="AB9" s="85"/>
-      <c r="AC9" s="85"/>
+      <c r="AB9" s="92"/>
+      <c r="AC9" s="92"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B10" s="29" t="s">
@@ -3134,8 +3134,8 @@
       </c>
     </row>
     <row r="24" spans="2:29" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AB24" s="88"/>
-      <c r="AC24" s="88"/>
+      <c r="AB24" s="87"/>
+      <c r="AC24" s="87"/>
     </row>
     <row r="25" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="36" t="s">
@@ -3237,15 +3237,15 @@
         <f>Y25/Y8</f>
         <v>0.34353240740740743</v>
       </c>
-      <c r="AB25" s="89">
+      <c r="AB25" s="90">
         <f t="shared" ref="AB25:AB31" si="3">Y25+W25+U25+S25+Q25+O25+M25+K25+I25+G25+E25+C25</f>
         <v>8904.3599999999988</v>
       </c>
-      <c r="AC25" s="90"/>
+      <c r="AC25" s="91"/>
     </row>
     <row r="26" spans="2:29" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AB26" s="85"/>
-      <c r="AC26" s="85"/>
+      <c r="AB26" s="92"/>
+      <c r="AC26" s="92"/>
     </row>
     <row r="27" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="38" t="s">
@@ -3759,8 +3759,8 @@
       </c>
     </row>
     <row r="38" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AB38" s="88"/>
-      <c r="AC38" s="88"/>
+      <c r="AB38" s="87"/>
+      <c r="AC38" s="87"/>
     </row>
     <row r="39" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="44" t="s">
@@ -3862,11 +3862,11 @@
         <f>Y39/Y8</f>
         <v>0.21931944444444446</v>
       </c>
-      <c r="AB39" s="91">
+      <c r="AB39" s="85">
         <f>Y39+W39+U39+S39+Q39+O39+M39+K39+I39+G39+E39+C39</f>
         <v>7445.9999999999991</v>
       </c>
-      <c r="AC39" s="92"/>
+      <c r="AC39" s="86"/>
     </row>
     <row r="40" spans="2:29" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D40" s="82"/>
@@ -3984,11 +3984,11 @@
         <f>Y41/Y8</f>
         <v>0.56285185185185194</v>
       </c>
-      <c r="AB41" s="91">
+      <c r="AB41" s="85">
         <f>Y41+W41+U41+S41+Q41+O41+M41+K41+I41+G41+E41+C41</f>
         <v>16350.360000000002</v>
       </c>
-      <c r="AC41" s="92"/>
+      <c r="AC41" s="86"/>
     </row>
     <row r="42" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="12"/>
@@ -4016,8 +4016,8 @@
       <c r="X42" s="12"/>
       <c r="Y42" s="12"/>
       <c r="Z42" s="12"/>
-      <c r="AB42" s="93"/>
-      <c r="AC42" s="93"/>
+      <c r="AB42" s="88"/>
+      <c r="AC42" s="88"/>
     </row>
     <row r="43" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="52" t="s">
@@ -4317,8 +4317,8 @@
       </c>
     </row>
     <row r="50" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AB50" s="88"/>
-      <c r="AC50" s="88"/>
+      <c r="AB50" s="87"/>
+      <c r="AC50" s="87"/>
     </row>
     <row r="51" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="50" t="s">
@@ -4420,15 +4420,15 @@
         <f>Y51/Y8</f>
         <v>0.40972222222222221</v>
       </c>
-      <c r="AB51" s="91">
+      <c r="AB51" s="85">
         <f>Y51+W51+U51+S51+Q51+O51+M51+K51+I51+G51+E51+C51</f>
         <v>10170</v>
       </c>
-      <c r="AC51" s="92"/>
+      <c r="AC51" s="86"/>
     </row>
     <row r="52" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AB52" s="93"/>
-      <c r="AC52" s="93"/>
+      <c r="AB52" s="88"/>
+      <c r="AC52" s="88"/>
     </row>
     <row r="53" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="64" t="s">
@@ -4530,19 +4530,19 @@
         <f>Y53/Y8</f>
         <v>0.97257407407407415</v>
       </c>
-      <c r="AB53" s="91">
+      <c r="AB53" s="85">
         <f>Y53+W53+U53+S53+Q53+O53+M53+K53+I53+G53+E53+C53</f>
         <v>26520.360000000008</v>
       </c>
-      <c r="AC53" s="92"/>
+      <c r="AC53" s="86"/>
     </row>
     <row r="54" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="AB54" s="94"/>
-      <c r="AC54" s="94"/>
+      <c r="AB54" s="89"/>
+      <c r="AC54" s="89"/>
     </row>
     <row r="55" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AB55" s="88"/>
-      <c r="AC55" s="88"/>
+      <c r="AB55" s="87"/>
+      <c r="AC55" s="87"/>
     </row>
     <row r="56" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="49" t="s">
@@ -4644,28 +4644,20 @@
         <f>Y56/Y8</f>
         <v>2.7425925925925826E-2</v>
       </c>
-      <c r="AB56" s="91">
+      <c r="AB56" s="85">
         <f>Y56+W56+U56+S56+Q56+O56+M56+K56+I56+G56+E56+C56</f>
         <v>599.6399999999976</v>
       </c>
-      <c r="AC56" s="92"/>
+      <c r="AC56" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="AB56:AC56"/>
-    <mergeCell ref="AB50:AC50"/>
-    <mergeCell ref="AB51:AC51"/>
-    <mergeCell ref="AB52:AC52"/>
-    <mergeCell ref="AB53:AC53"/>
-    <mergeCell ref="AB54:AC54"/>
-    <mergeCell ref="AB55:AC55"/>
-    <mergeCell ref="AB38:AC38"/>
-    <mergeCell ref="AB39:AC39"/>
-    <mergeCell ref="AB42:AC42"/>
-    <mergeCell ref="AB41:AC41"/>
-    <mergeCell ref="AB24:AC24"/>
-    <mergeCell ref="AB25:AC25"/>
-    <mergeCell ref="AB26:AC26"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="AB9:AC9"/>
     <mergeCell ref="AB3:AC3"/>
     <mergeCell ref="AB7:AC7"/>
@@ -4676,12 +4668,20 @@
     <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="AB38:AC38"/>
+    <mergeCell ref="AB39:AC39"/>
+    <mergeCell ref="AB42:AC42"/>
+    <mergeCell ref="AB41:AC41"/>
+    <mergeCell ref="AB24:AC24"/>
+    <mergeCell ref="AB25:AC25"/>
+    <mergeCell ref="AB26:AC26"/>
+    <mergeCell ref="AB56:AC56"/>
+    <mergeCell ref="AB50:AC50"/>
+    <mergeCell ref="AB51:AC51"/>
+    <mergeCell ref="AB52:AC52"/>
+    <mergeCell ref="AB53:AC53"/>
+    <mergeCell ref="AB54:AC54"/>
+    <mergeCell ref="AB55:AC55"/>
   </mergeCells>
   <conditionalFormatting sqref="AC4:AC6">
     <cfRule type="colorScale" priority="13">

</xml_diff>